<commit_message>
Fixing issues relating to energy efficiency values above 1 for certain activities
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-synfuels-from-FT-from-coal-gasification.xlsx
+++ b/premise/data/additional_inventories/lci-synfuels-from-FT-from-coal-gasification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27255" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-27252" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="FT fuel - Diesel" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="101">
   <si>
     <t>Activity</t>
   </si>
@@ -734,20 +734,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K575"/>
+  <dimension ref="A1:K574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="B226" sqref="B226"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -755,10 +755,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -766,7 +766,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -774,7 +774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -782,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
@@ -790,7 +790,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
@@ -798,7 +798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
@@ -806,12 +806,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>94</v>
       </c>
@@ -875,7 +875,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>83</v>
       </c>
@@ -900,7 +900,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
@@ -925,7 +925,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>61</v>
       </c>
@@ -950,7 +950,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>63</v>
       </c>
@@ -975,7 +975,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>65</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>67</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>69</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>71</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>73</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>76</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>80</v>
       </c>
@@ -1150,12 +1150,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="16"/>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>7</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>1</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>2</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>3</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>5</v>
       </c>
@@ -1203,12 +1203,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>11</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>95</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>84</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>27</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>61</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>63</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>65</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>67</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>69</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>71</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>73</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>76</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>80</v>
       </c>
@@ -1547,12 +1547,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
       <c r="B44" s="16"/>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>7</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>1</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>2</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>3</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>5</v>
       </c>
@@ -1600,12 +1600,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>11</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>96</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>85</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>27</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>61</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>63</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>65</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>67</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>69</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>71</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>73</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>76</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>80</v>
       </c>
@@ -1944,12 +1944,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="B65" s="16"/>
       <c r="G65" s="12"/>
     </row>
-    <row r="66" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>0</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
         <v>7</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>1</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
         <v>2</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>3</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>5</v>
       </c>
@@ -1997,12 +1997,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
         <v>11</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>97</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>86</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
         <v>27</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
         <v>61</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="s">
         <v>63</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
         <v>65</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
         <v>67</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="s">
         <v>69</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="s">
         <v>71</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
         <v>73</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
         <v>76</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
         <v>80</v>
       </c>
@@ -2341,12 +2341,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="12"/>
       <c r="B86" s="16"/>
       <c r="G86" s="12"/>
     </row>
-    <row r="87" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>0</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
         <v>1</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
         <v>2</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
         <v>3</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
         <v>5</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
         <v>7</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
         <v>9</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
         <v>38</v>
       </c>
@@ -2410,12 +2410,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
         <v>11</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
         <v>83</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
         <v>93</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="s">
         <v>19</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
         <v>24</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="10" t="s">
         <v>41</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
         <v>27</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="s">
         <v>100</v>
       </c>
@@ -2599,8 +2599,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
         <v>0</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="9" t="s">
         <v>1</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="9" t="s">
         <v>2</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="108" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="9" t="s">
         <v>3</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="9" t="s">
         <v>5</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="9" t="s">
         <v>7</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="9" t="s">
         <v>9</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="9" t="s">
         <v>38</v>
       </c>
@@ -2664,12 +2664,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="113" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="9" t="s">
         <v>11</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="10" t="s">
         <v>87</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="9" t="s">
         <v>93</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="117" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="9" t="s">
         <v>19</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="9" t="s">
         <v>24</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="10" t="s">
         <v>41</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="120" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="9" t="s">
         <v>27</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="9" t="s">
         <v>100</v>
       </c>
@@ -2850,8 +2850,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="7" t="s">
         <v>0</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="9" t="s">
         <v>1</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="9" t="s">
         <v>2</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="126" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="9" t="s">
         <v>3</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="9" t="s">
         <v>5</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="9" t="s">
         <v>7</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="9" t="s">
         <v>9</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="130" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="9" t="s">
         <v>38</v>
       </c>
@@ -2915,12 +2915,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="9" t="s">
         <v>11</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="10" t="s">
         <v>84</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="9" t="s">
         <v>93</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="135" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="9" t="s">
         <v>19</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="9" t="s">
         <v>24</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="10" t="s">
         <v>41</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="138" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="9" t="s">
         <v>27</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="139" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="9" t="s">
         <v>100</v>
       </c>
@@ -3104,8 +3104,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>0</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="9" t="s">
         <v>1</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="9" t="s">
         <v>2</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="144" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="9" t="s">
         <v>3</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="9" t="s">
         <v>5</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="9" t="s">
         <v>7</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="9" t="s">
         <v>9</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="148" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="9" t="s">
         <v>38</v>
       </c>
@@ -3169,12 +3169,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="149" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="9" t="s">
         <v>11</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="10" t="s">
         <v>88</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="9" t="s">
         <v>93</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="153" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="9" t="s">
         <v>19</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="154" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="9" t="s">
         <v>24</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="10" t="s">
         <v>41</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="156" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="9" t="s">
         <v>27</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="157" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="9" t="s">
         <v>98</v>
       </c>
@@ -3358,10 +3358,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B158" s="11"/>
     </row>
-    <row r="159" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="7" t="s">
         <v>0</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="160" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="9" t="s">
         <v>1</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="9" t="s">
         <v>2</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="162" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="9" t="s">
         <v>3</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="9" t="s">
         <v>5</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="9" t="s">
         <v>7</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="9" t="s">
         <v>9</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="166" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="9" t="s">
         <v>38</v>
       </c>
@@ -3425,12 +3425,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="167" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="9" t="s">
         <v>11</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="10" t="s">
         <v>85</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="9" t="s">
         <v>93</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="171" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="9" t="s">
         <v>19</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="172" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="9" t="s">
         <v>24</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="173" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="10" t="s">
         <v>41</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="174" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="9" t="s">
         <v>27</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="175" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="9" t="s">
         <v>98</v>
       </c>
@@ -3614,8 +3614,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="176" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="177" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="7" t="s">
         <v>0</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="178" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="9" t="s">
         <v>1</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="9" t="s">
         <v>2</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="180" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="9" t="s">
         <v>3</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="9" t="s">
         <v>5</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="9" t="s">
         <v>7</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="9" t="s">
         <v>9</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="184" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="9" t="s">
         <v>38</v>
       </c>
@@ -3679,12 +3679,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="185" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="9" t="s">
         <v>11</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="10" t="s">
         <v>89</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="188" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="9" t="s">
         <v>93</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="189" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="9" t="s">
         <v>19</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="190" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="9" t="s">
         <v>24</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="191" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="10" t="s">
         <v>41</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="192" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="9" t="s">
         <v>27</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="9" t="s">
         <v>100</v>
       </c>
@@ -3865,8 +3865,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="194" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="195" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
         <v>0</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="196" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="9" t="s">
         <v>1</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="9" t="s">
         <v>2</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="9" t="s">
         <v>3</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="9" t="s">
         <v>5</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="200" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="9" t="s">
         <v>7</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="9" t="s">
         <v>9</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="202" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="9" t="s">
         <v>38</v>
       </c>
@@ -3930,12 +3930,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="203" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A203" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="9" t="s">
         <v>11</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="10" t="s">
         <v>86</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="206" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="9" t="s">
         <v>93</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="207" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="9" t="s">
         <v>19</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="208" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="9" t="s">
         <v>24</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="209" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="10" t="s">
         <v>41</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="210" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="9" t="s">
         <v>27</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="211" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="9" t="s">
         <v>100</v>
       </c>
@@ -4119,8 +4119,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="213" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="213" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
         <v>0</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="214" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="9" t="s">
         <v>1</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="9" t="s">
         <v>2</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="216" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="9" t="s">
         <v>3</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="9" t="s">
         <v>5</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="218" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="9" t="s">
         <v>7</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="9" t="s">
         <v>9</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="220" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="9" t="s">
         <v>38</v>
       </c>
@@ -4184,12 +4184,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="221" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A221" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="9" t="s">
         <v>11</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="9" t="s">
         <v>92</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="224" spans="1:8" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A224" s="12" t="s">
         <v>90</v>
       </c>
@@ -4252,620 +4252,600 @@
         <v>91</v>
       </c>
     </row>
-    <row r="225" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B225" s="9">
-        <v>0.36599999999999999</v>
-      </c>
-      <c r="C225" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D225" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F225" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G225" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B226" s="9">
         <f>60*0.001/106.6</f>
         <v>5.6285178236397749E-4</v>
       </c>
+      <c r="D225" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E225" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F225" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B226" s="9">
+        <v>1</v>
+      </c>
+      <c r="C226" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="D226" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E226" s="9" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F226" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G226" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B227" s="9">
+        <v>32</v>
+      </c>
+      <c r="B227" s="13">
+        <v>5.7100000000000004E-6</v>
+      </c>
+      <c r="C227" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D227" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F227" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B228" s="13"/>
+    </row>
+    <row r="229" spans="1:7" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A229" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C227" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D227" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F227" s="9" t="s">
+      <c r="B230" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B231" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B232" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B233" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B234" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B235" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A236" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B237" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C237" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D237" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E237" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F237" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G237" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B238" s="9">
+        <v>1</v>
+      </c>
+      <c r="C238" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D238" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F238" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G227" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="228" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B228" s="13">
-        <v>5.7100000000000004E-6</v>
-      </c>
-      <c r="C228" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D228" s="9" t="s">
+      <c r="G238" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A239" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B239" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C239" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D239" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F239" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G239" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A240" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B240" s="9">
+        <v>1.57</v>
+      </c>
+      <c r="C240" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D240" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F240" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G240" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A241" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B241" s="11">
+        <v>1.9300000000000002E-9</v>
+      </c>
+      <c r="C241" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D241" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F228" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="229" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B229" s="13"/>
-    </row>
-    <row r="230" spans="1:7" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A230" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B230" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="231" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B231" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B232" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="233" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B233" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="234" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B234" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="235" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B235" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="236" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B236" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="237" spans="1:7" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A237" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="238" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B238" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C238" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D238" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E238" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F238" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G238" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="239" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B239" s="9">
-        <v>1</v>
-      </c>
-      <c r="C239" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D239" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F239" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G239" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="240" spans="1:7" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A240" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B240" s="9">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C240" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D240" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F240" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G240" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A241" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B241" s="9">
-        <v>1.57</v>
-      </c>
-      <c r="C241" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D241" s="9" t="s">
-        <v>6</v>
-      </c>
       <c r="F241" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G241" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="242" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B242" s="11">
-        <v>1.9300000000000002E-9</v>
-      </c>
-      <c r="C242" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D242" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F242" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G242" s="10" t="s">
+      <c r="G241" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="243" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="10"/>
-      <c r="B243" s="11"/>
-      <c r="G243" s="10"/>
-    </row>
-    <row r="245" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A245" s="1"/>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A242" s="10"/>
+      <c r="B242" s="11"/>
+      <c r="G242" s="10"/>
+    </row>
+    <row r="244" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A244" s="1"/>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B250" s="3"/>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B251" s="3"/>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B252" s="3"/>
-    </row>
-    <row r="254" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A254" s="1"/>
-      <c r="B254" s="2"/>
-    </row>
-    <row r="261" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A261" s="1"/>
-    </row>
-    <row r="264" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A264" s="4"/>
-      <c r="G264" s="4"/>
-    </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A253" s="1"/>
+      <c r="B253" s="2"/>
+    </row>
+    <row r="260" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A260" s="1"/>
+    </row>
+    <row r="263" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A263" s="4"/>
+      <c r="G263" s="4"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B267" s="5"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B268" s="5"/>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B269" s="5"/>
-    </row>
-    <row r="270" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A270" s="1"/>
-      <c r="B270" s="2"/>
-    </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B272" s="6"/>
-    </row>
-    <row r="277" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A277" s="1"/>
-    </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A279" s="6"/>
-      <c r="G279" s="6"/>
-    </row>
-    <row r="280" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A269" s="1"/>
+      <c r="B269" s="2"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B271" s="6"/>
+    </row>
+    <row r="276" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A276" s="1"/>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A278" s="6"/>
+      <c r="G278" s="6"/>
+    </row>
+    <row r="279" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A279" s="4"/>
+      <c r="G279" s="4"/>
+    </row>
+    <row r="280" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A280" s="4"/>
       <c r="G280" s="4"/>
     </row>
-    <row r="281" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A281" s="4"/>
-      <c r="G281" s="4"/>
-    </row>
-    <row r="284" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A284" s="1"/>
-      <c r="B284" s="2"/>
-    </row>
-    <row r="291" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A291" s="1"/>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A283" s="1"/>
+      <c r="B283" s="2"/>
+    </row>
+    <row r="290" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A290" s="1"/>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B296" s="3"/>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B297" s="3"/>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B298" s="3"/>
-    </row>
-    <row r="300" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A300" s="1"/>
-      <c r="B300" s="2"/>
-    </row>
-    <row r="307" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A307" s="1"/>
-    </row>
-    <row r="310" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A310" s="4"/>
-      <c r="G310" s="4"/>
-    </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A299" s="1"/>
+      <c r="B299" s="2"/>
+    </row>
+    <row r="306" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A306" s="1"/>
+    </row>
+    <row r="309" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A309" s="4"/>
+      <c r="G309" s="4"/>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B313" s="5"/>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B314" s="5"/>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B315" s="5"/>
-    </row>
-    <row r="316" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A316" s="1"/>
-      <c r="B316" s="2"/>
-    </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B318" s="6"/>
-    </row>
-    <row r="323" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A323" s="1"/>
-    </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A325" s="6"/>
-      <c r="G325" s="6"/>
-    </row>
-    <row r="326" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A315" s="1"/>
+      <c r="B315" s="2"/>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B317" s="6"/>
+    </row>
+    <row r="322" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A322" s="1"/>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A324" s="6"/>
+      <c r="G324" s="6"/>
+    </row>
+    <row r="325" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A325" s="4"/>
+      <c r="G325" s="4"/>
+    </row>
+    <row r="326" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A326" s="4"/>
       <c r="G326" s="4"/>
     </row>
-    <row r="327" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A327" s="4"/>
-      <c r="G327" s="4"/>
-    </row>
-    <row r="330" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A330" s="1"/>
-      <c r="B330" s="2"/>
-    </row>
-    <row r="337" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A337" s="1"/>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A329" s="1"/>
+      <c r="B329" s="2"/>
+    </row>
+    <row r="336" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A336" s="1"/>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B342" s="3"/>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B343" s="3"/>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B344" s="3"/>
-    </row>
-    <row r="346" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A346" s="1"/>
-      <c r="B346" s="2"/>
-    </row>
-    <row r="353" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A353" s="1"/>
-    </row>
-    <row r="356" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A356" s="4"/>
-      <c r="G356" s="4"/>
-    </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A345" s="1"/>
+      <c r="B345" s="2"/>
+    </row>
+    <row r="352" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A352" s="1"/>
+    </row>
+    <row r="355" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A355" s="4"/>
+      <c r="G355" s="4"/>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B359" s="5"/>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B360" s="5"/>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B361" s="5"/>
-    </row>
-    <row r="362" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A362" s="1"/>
-      <c r="B362" s="2"/>
-    </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B364" s="6"/>
-    </row>
-    <row r="369" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A369" s="1"/>
-    </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A371" s="6"/>
-      <c r="G371" s="6"/>
-    </row>
-    <row r="372" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A361" s="1"/>
+      <c r="B361" s="2"/>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B363" s="6"/>
+    </row>
+    <row r="368" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A368" s="1"/>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A370" s="6"/>
+      <c r="G370" s="6"/>
+    </row>
+    <row r="371" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A371" s="4"/>
+      <c r="G371" s="4"/>
+    </row>
+    <row r="372" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A372" s="4"/>
       <c r="G372" s="4"/>
     </row>
-    <row r="373" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A373" s="4"/>
-      <c r="G373" s="4"/>
-    </row>
-    <row r="376" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A376" s="1"/>
-      <c r="B376" s="2"/>
-    </row>
-    <row r="383" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A383" s="1"/>
-    </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A375" s="1"/>
+      <c r="B375" s="2"/>
+    </row>
+    <row r="382" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A382" s="1"/>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B388" s="3"/>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B389" s="3"/>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B390" s="3"/>
-    </row>
-    <row r="392" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A392" s="1"/>
-      <c r="B392" s="2"/>
-    </row>
-    <row r="399" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A399" s="1"/>
-    </row>
-    <row r="402" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A402" s="4"/>
-      <c r="G402" s="4"/>
-    </row>
-    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A391" s="1"/>
+      <c r="B391" s="2"/>
+    </row>
+    <row r="398" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A398" s="1"/>
+    </row>
+    <row r="401" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A401" s="4"/>
+      <c r="G401" s="4"/>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B405" s="5"/>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B406" s="5"/>
     </row>
-    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B407" s="5"/>
-    </row>
-    <row r="408" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A408" s="1"/>
-      <c r="B408" s="2"/>
-    </row>
-    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B410" s="6"/>
-    </row>
-    <row r="415" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A415" s="1"/>
-    </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A417" s="6"/>
-      <c r="G417" s="6"/>
-    </row>
-    <row r="418" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A407" s="1"/>
+      <c r="B407" s="2"/>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B409" s="6"/>
+    </row>
+    <row r="414" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A414" s="1"/>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A416" s="6"/>
+      <c r="G416" s="6"/>
+    </row>
+    <row r="417" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A417" s="4"/>
+      <c r="G417" s="4"/>
+    </row>
+    <row r="418" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A418" s="4"/>
       <c r="G418" s="4"/>
     </row>
-    <row r="419" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A419" s="4"/>
-      <c r="G419" s="4"/>
-    </row>
-    <row r="422" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A422" s="1"/>
-      <c r="B422" s="2"/>
-    </row>
-    <row r="429" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A429" s="1"/>
-    </row>
-    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A421" s="1"/>
+      <c r="B421" s="2"/>
+    </row>
+    <row r="428" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A428" s="1"/>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B434" s="3"/>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B435" s="3"/>
     </row>
-    <row r="436" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B436" s="3"/>
-    </row>
-    <row r="438" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A438" s="1"/>
-      <c r="B438" s="2"/>
-    </row>
-    <row r="445" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A445" s="1"/>
-    </row>
-    <row r="448" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A448" s="4"/>
-      <c r="G448" s="4"/>
-    </row>
-    <row r="452" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B452" s="5"/>
-    </row>
-    <row r="454" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A454" s="1"/>
-      <c r="B454" s="2"/>
-    </row>
-    <row r="456" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B456" s="6"/>
-    </row>
-    <row r="461" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A461" s="1"/>
-    </row>
-    <row r="463" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A463" s="6"/>
-      <c r="G463" s="6"/>
-    </row>
-    <row r="464" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A437" s="1"/>
+      <c r="B437" s="2"/>
+    </row>
+    <row r="444" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A444" s="1"/>
+    </row>
+    <row r="447" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A447" s="4"/>
+      <c r="G447" s="4"/>
+    </row>
+    <row r="451" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B451" s="5"/>
+    </row>
+    <row r="453" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A453" s="1"/>
+      <c r="B453" s="2"/>
+    </row>
+    <row r="455" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B455" s="6"/>
+    </row>
+    <row r="460" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A460" s="1"/>
+    </row>
+    <row r="462" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A462" s="6"/>
+      <c r="G462" s="6"/>
+    </row>
+    <row r="463" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A463" s="4"/>
+      <c r="G463" s="4"/>
+    </row>
+    <row r="464" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A464" s="4"/>
       <c r="G464" s="4"/>
     </row>
-    <row r="465" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A465" s="4"/>
-      <c r="G465" s="4"/>
-    </row>
-    <row r="467" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A467" s="1"/>
-      <c r="B467" s="2"/>
-    </row>
-    <row r="474" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A474" s="1"/>
-    </row>
-    <row r="480" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A466" s="1"/>
+      <c r="B466" s="2"/>
+    </row>
+    <row r="473" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A473" s="1"/>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B479" s="3"/>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B480" s="3"/>
     </row>
-    <row r="481" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B481" s="3"/>
-    </row>
-    <row r="483" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A483" s="1"/>
-      <c r="B483" s="2"/>
-    </row>
-    <row r="490" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A490" s="1"/>
-    </row>
-    <row r="493" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A493" s="4"/>
-      <c r="G493" s="4"/>
-    </row>
-    <row r="497" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A482" s="1"/>
+      <c r="B482" s="2"/>
+    </row>
+    <row r="489" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A489" s="1"/>
+    </row>
+    <row r="492" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A492" s="4"/>
+      <c r="G492" s="4"/>
+    </row>
+    <row r="496" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B496" s="5"/>
+    </row>
+    <row r="497" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B497" s="5"/>
     </row>
-    <row r="498" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B498" s="5"/>
-    </row>
-    <row r="499" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A499" s="1"/>
-      <c r="B499" s="2"/>
-    </row>
-    <row r="501" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B501" s="6"/>
-    </row>
-    <row r="506" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A506" s="1"/>
-    </row>
-    <row r="508" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A508" s="6"/>
-      <c r="G508" s="6"/>
-    </row>
-    <row r="509" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A498" s="1"/>
+      <c r="B498" s="2"/>
+    </row>
+    <row r="500" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B500" s="6"/>
+    </row>
+    <row r="505" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A505" s="1"/>
+    </row>
+    <row r="507" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A507" s="6"/>
+      <c r="G507" s="6"/>
+    </row>
+    <row r="508" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A508" s="4"/>
+      <c r="G508" s="4"/>
+    </row>
+    <row r="509" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A509" s="4"/>
       <c r="G509" s="4"/>
     </row>
-    <row r="510" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A510" s="4"/>
-      <c r="G510" s="4"/>
-    </row>
-    <row r="513" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A513" s="1"/>
-      <c r="B513" s="2"/>
-    </row>
-    <row r="520" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A520" s="1"/>
-    </row>
-    <row r="526" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A512" s="1"/>
+      <c r="B512" s="2"/>
+    </row>
+    <row r="519" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A519" s="1"/>
+    </row>
+    <row r="525" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B525" s="3"/>
+    </row>
+    <row r="526" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B526" s="3"/>
     </row>
-    <row r="527" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B527" s="3"/>
-    </row>
-    <row r="529" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A529" s="1"/>
-      <c r="B529" s="2"/>
-    </row>
-    <row r="536" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A536" s="1"/>
-    </row>
-    <row r="539" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A539" s="4"/>
-      <c r="G539" s="4"/>
-    </row>
-    <row r="543" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B543" s="5"/>
-    </row>
-    <row r="545" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A545" s="1"/>
-      <c r="B545" s="2"/>
-    </row>
-    <row r="547" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B547" s="6"/>
-    </row>
-    <row r="552" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A552" s="1"/>
-    </row>
-    <row r="554" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A554" s="6"/>
-      <c r="G554" s="6"/>
-    </row>
-    <row r="555" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A528" s="1"/>
+      <c r="B528" s="2"/>
+    </row>
+    <row r="535" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A535" s="1"/>
+    </row>
+    <row r="538" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A538" s="4"/>
+      <c r="G538" s="4"/>
+    </row>
+    <row r="542" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B542" s="5"/>
+    </row>
+    <row r="544" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A544" s="1"/>
+      <c r="B544" s="2"/>
+    </row>
+    <row r="546" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B546" s="6"/>
+    </row>
+    <row r="551" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A551" s="1"/>
+    </row>
+    <row r="553" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A553" s="6"/>
+      <c r="G553" s="6"/>
+    </row>
+    <row r="554" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A554" s="4"/>
+      <c r="G554" s="4"/>
+    </row>
+    <row r="555" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A555" s="4"/>
       <c r="G555" s="4"/>
     </row>
-    <row r="556" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A556" s="4"/>
-      <c r="G556" s="4"/>
-    </row>
-    <row r="558" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A558" s="1"/>
-      <c r="B558" s="2"/>
-    </row>
-    <row r="564" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A564" s="1"/>
-    </row>
-    <row r="569" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A569" s="1"/>
-      <c r="B569" s="2"/>
-    </row>
-    <row r="575" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A575" s="1"/>
+    <row r="557" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A557" s="1"/>
+      <c r="B557" s="2"/>
+    </row>
+    <row r="563" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A563" s="1"/>
+    </row>
+    <row r="568" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A568" s="1"/>
+      <c r="B568" s="2"/>
+    </row>
+    <row r="574" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A574" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>